<commit_message>
[WIP] remove field from mapping, use key instead. perpare for products import + attributes
</commit_message>
<xml_diff>
--- a/Resources/Private/ExampleData/categoriesxls.xlsx
+++ b/Resources/Private/ExampleData/categoriesxls.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
   <si>
     <t xml:space="preserve">Import ID</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">Produkter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roadsters</t>
   </si>
 </sst>
 </file>
@@ -67,7 +70,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -127,12 +129,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -153,18 +151,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -186,13 +184,13 @@
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="0" t="s">
         <v>6</v>
       </c>
     </row>
@@ -200,13 +198,13 @@
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="0" t="s">
         <v>4</v>
       </c>
     </row>
@@ -220,7 +218,7 @@
       <c r="C4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="0" t="s">
         <v>6</v>
       </c>
     </row>
@@ -233,6 +231,20 @@
       </c>
       <c r="C5" s="0" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>